<commit_message>
arquivos atualizados + .gitignore adicionado
</commit_message>
<xml_diff>
--- a/Modelagens/Locadora/Modelagem-Fisico.xlsx
+++ b/Modelagens/Locadora/Modelagem-Fisico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49549303837\Desktop\DB\Senai-2Semestre-DB\Modelagens\Locadora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1962E29F-8607-4151-8A88-D19D64971EBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A290E86-EB26-4E27-898D-03E920CCBA5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{A158423D-3023-4F3D-85AD-27713970E8CC}"/>
   </bookViews>
@@ -358,8 +358,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -378,7 +381,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -403,19 +405,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,41 +729,46 @@
   <dimension ref="B1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="1"/>
+    <col min="20" max="20" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
@@ -783,19 +783,19 @@
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="14"/>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="18"/>
-      <c r="Q5" s="16" t="s">
+      <c r="N5" s="15"/>
+      <c r="O5" s="14"/>
+      <c r="Q5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="18"/>
-      <c r="T5" s="16" t="s">
+      <c r="R5" s="14"/>
+      <c r="T5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="18"/>
+      <c r="U5" s="14"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
@@ -990,7 +990,7 @@
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="19"/>
+      <c r="F10" s="16"/>
       <c r="I10" s="12">
         <v>4</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="T11" s="12">
         <v>5</v>
       </c>
-      <c r="U11" s="7" t="s">
+      <c r="U11" s="8" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1215,7 +1215,7 @@
       <c r="C21" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="P21" s="20"/>
+      <c r="P21" s="17"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="12">
@@ -1226,8 +1226,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="I1:K2"/>

</xml_diff>